<commit_message>
more and more footprints
</commit_message>
<xml_diff>
--- a/KiCad documents/HybridChargeController-Orderlist.xlsx
+++ b/KiCad documents/HybridChargeController-Orderlist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/538aba7ce6d818b8/Documents/Arbeit/MEI/Hybrid Charge controller/KiCad documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koops\OneDrive\Documents\Arbeit\MEI\Hybrid Charge controller\KiCad documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -222,10 +222,10 @@
     <t>Auf Lager</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>MMBT3904</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1070,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1203,7 +1203,7 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -1217,7 +1217,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -1231,7 +1231,7 @@
         <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -1256,10 +1256,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
         <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -1287,7 +1287,7 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -1301,7 +1301,7 @@
         <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -1315,7 +1315,7 @@
         <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -1329,7 +1329,7 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
@@ -1343,7 +1343,7 @@
         <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -1371,7 +1371,7 @@
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -1483,7 +1483,7 @@
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
@@ -1497,7 +1497,7 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
@@ -1525,7 +1525,7 @@
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>